<commit_message>
- added example units listbox in row 2 that is populated from sheet named units - create example data for example user with which to show off dashboard functionality: give initial data point and make data traverse a random walk stepping within 25% up or down every step
</commit_message>
<xml_diff>
--- a/fegs-cs-data-into-table-madness.xlsx
+++ b/fegs-cs-data-into-table-madness.xlsx
@@ -13,8 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="fegs-cs-data" sheetId="1" r:id="rId1"/>
-    <sheet name="user-interface" sheetId="2" r:id="rId2"/>
-    <sheet name="possible metrics" sheetId="3" r:id="rId3"/>
+    <sheet name="units" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7695" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7696" uniqueCount="398">
   <si>
     <t>Environmental Class</t>
   </si>
@@ -1198,25 +1197,28 @@
     <t>water (from precipitation) suitable for drinking (i.e., human consumption), specifically via cisterns</t>
   </si>
   <si>
-    <t>user-interface</t>
-  </si>
-  <si>
-    <t>possible metrics</t>
-  </si>
-  <si>
-    <t>user's suggested metrics</t>
-  </si>
-  <si>
-    <t>blah, blahh, blahtoo, blahAsWell</t>
-  </si>
-  <si>
-    <t>metric</t>
-  </si>
-  <si>
     <t>measured value</t>
   </si>
   <si>
-    <t>foo, fooToo</t>
+    <t>units</t>
+  </si>
+  <si>
+    <t>write in possible units(one per cell) to populate the units field's listbox of corresponding row of fegs-cs</t>
+  </si>
+  <si>
+    <t>mg/day</t>
+  </si>
+  <si>
+    <t>ft^3/s</t>
+  </si>
+  <si>
+    <t>a second unit to populate listbox</t>
+  </si>
+  <si>
+    <t>a third unit which will populate the listbox</t>
+  </si>
+  <si>
+    <t>TEST WITH ME!</t>
   </si>
 </sst>
 </file>
@@ -1232,12 +1234,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1252,8 +1260,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1272,9 +1284,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:R560" totalsRowShown="0">
-  <autoFilter ref="A1:R560"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P560" totalsRowShown="0">
+  <autoFilter ref="A1:P560"/>
+  <tableColumns count="16">
     <tableColumn id="1" name="Environmental Class"/>
     <tableColumn id="2" name="Environmental Subclass"/>
     <tableColumn id="3" name="Beneficiary Category"/>
@@ -1289,10 +1301,8 @@
     <tableColumn id="12" name="Status"/>
     <tableColumn id="13" name="Source"/>
     <tableColumn id="14" name="Notes"/>
-    <tableColumn id="17" name="metric"/>
+    <tableColumn id="17" name="units"/>
     <tableColumn id="20" name="measured value"/>
-    <tableColumn id="15" name="possible metrics"/>
-    <tableColumn id="16" name="user's suggested metrics"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1561,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R560"/>
+  <dimension ref="A1:P560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,21 +1582,19 @@
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="37.140625" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" customWidth="1"/>
     <col min="14" max="15" width="14.85546875" customWidth="1"/>
     <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1630,19 +1638,13 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="P1" t="s">
-        <v>395</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>391</v>
-      </c>
-      <c r="R1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1685,17 +1687,14 @@
       <c r="N2" t="s">
         <v>25</v>
       </c>
+      <c r="O2" s="2" t="s">
+        <v>397</v>
+      </c>
       <c r="P2" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" t="s">
-        <v>393</v>
-      </c>
-      <c r="R2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1742,7 +1741,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1789,7 +1788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1836,7 +1835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1883,7 +1882,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1930,7 +1929,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2024,7 +2023,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2165,7 +2164,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2212,7 +2211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2259,7 +2258,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -27926,42 +27925,56 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>units!2:2</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>390</v>
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B2" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>